<commit_message>
Integration saisie paramètres de marché
duplicatin de code saisie Intrinsèque et adaptation dans saisie marché
</commit_message>
<xml_diff>
--- a/module classe projet/ModulePrincipal/Parametres.xlsx
+++ b/module classe projet/ModulePrincipal/Parametres.xlsx
@@ -7,6 +7,7 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Int couts" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Mar couts" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -14,11 +15,86 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="32">
   <si>
     <t xml:space="preserve">Prestation de cours </t>
   </si>
   <si>
+    <t>Couts d'assurance</t>
+  </si>
+  <si>
+    <t>Autres assurances (MAD)</t>
+  </si>
+  <si>
+    <t>Cout Assurances=0</t>
+  </si>
+  <si>
+    <t>Horizon=0</t>
+  </si>
+  <si>
+    <t>Horizon=1</t>
+  </si>
+  <si>
+    <t>Horizon=2</t>
+  </si>
+  <si>
+    <t>Horizon=3</t>
+  </si>
+  <si>
+    <t>Horizon=4</t>
+  </si>
+  <si>
+    <t>Cout de location, espace</t>
+  </si>
+  <si>
+    <t>Nombre espaces loués</t>
+  </si>
+  <si>
+    <t>Espace=0</t>
+  </si>
+  <si>
+    <t>Espace=1</t>
+  </si>
+  <si>
+    <t>Espace=2</t>
+  </si>
+  <si>
+    <t>Espace=3</t>
+  </si>
+  <si>
+    <t>Espace=4</t>
+  </si>
+  <si>
+    <t>Cout d'energie, électricité</t>
+  </si>
+  <si>
+    <t>Nombre de postes de consommation électriques</t>
+  </si>
+  <si>
+    <t>Poste=0</t>
+  </si>
+  <si>
+    <t>Poste=1</t>
+  </si>
+  <si>
+    <t>Poste=2</t>
+  </si>
+  <si>
+    <t>Poste=3</t>
+  </si>
+  <si>
+    <t>Poste=4</t>
+  </si>
+  <si>
+    <t>Poste=5</t>
+  </si>
+  <si>
+    <t>Consommation Electrique par poste ( Kwh )</t>
+  </si>
+  <si>
+    <t>Consommation Electrique par poste ( MAD )</t>
+  </si>
+  <si>
     <t>Cout d'entretien</t>
   </si>
   <si>
@@ -28,79 +104,13 @@
     <t>Cout Maintenance=0</t>
   </si>
   <si>
-    <t>Horizon=0</t>
-  </si>
-  <si>
-    <t>Horizon=1</t>
-  </si>
-  <si>
-    <t>Horizon=2</t>
-  </si>
-  <si>
-    <t>Horizon=3</t>
-  </si>
-  <si>
-    <t>Horizon=4</t>
-  </si>
-  <si>
-    <t>Cout d'energie, électricité</t>
-  </si>
-  <si>
-    <t>Nombre de postes de consommation électriques</t>
-  </si>
-  <si>
-    <t>Poste=0</t>
-  </si>
-  <si>
-    <t>Poste=1</t>
-  </si>
-  <si>
-    <t>Poste=2</t>
-  </si>
-  <si>
-    <t>Poste=3</t>
-  </si>
-  <si>
-    <t>Poste=4</t>
-  </si>
-  <si>
-    <t>Poste=5</t>
-  </si>
-  <si>
-    <t>Consommation Electrique par poste ( Kwh )</t>
-  </si>
-  <si>
-    <t>Consommation Electrique par poste ( MAD )</t>
-  </si>
-  <si>
-    <t>Cout de location, espace</t>
-  </si>
-  <si>
-    <t>Nombre espaces loués</t>
-  </si>
-  <si>
-    <t>Espace=0</t>
-  </si>
-  <si>
-    <t>Espace=1</t>
-  </si>
-  <si>
-    <t>Espace=2</t>
-  </si>
-  <si>
-    <t>Espace=3</t>
-  </si>
-  <si>
-    <t>Espace=4</t>
-  </si>
-  <si>
-    <t>Couts d'assurance</t>
-  </si>
-  <si>
-    <t>Autres assurances (MAD)</t>
-  </si>
-  <si>
-    <t>Cout Assurances=0</t>
+    <t>Prix de Location</t>
+  </si>
+  <si>
+    <t>Prix du Kwh</t>
+  </si>
+  <si>
+    <t>Cout Kwh=0</t>
   </si>
 </sst>
 </file>
@@ -591,9 +601,6 @@
       <c r="K16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L16" s="1" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="17" spans="1:12">
       <c r="F17" s="1" t="s">
@@ -614,9 +621,6 @@
       <c r="K17" t="n">
         <v>0</v>
       </c>
-      <c r="L17" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="18" spans="1:12">
       <c r="F18" s="1" t="s">
@@ -637,9 +641,6 @@
       <c r="K18" t="n">
         <v>0</v>
       </c>
-      <c r="L18" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="19" spans="1:12">
       <c r="F19" s="1" t="s">
@@ -660,9 +661,6 @@
       <c r="K19" t="n">
         <v>0</v>
       </c>
-      <c r="L19" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="20" spans="1:12">
       <c r="F20" s="1" t="s">
@@ -683,9 +681,6 @@
       <c r="K20" t="n">
         <v>0</v>
       </c>
-      <c r="L20" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="21" spans="1:12">
       <c r="F21" s="1" t="s">
@@ -706,12 +701,13 @@
       <c r="K21" t="n">
         <v>0</v>
       </c>
-      <c r="L21" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="22" spans="1:12"/>
-    <row r="23" spans="1:12"/>
+    <row r="23" spans="1:12">
+      <c r="E23" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="24" spans="1:12"/>
     <row r="25" spans="1:12"/>
     <row r="26" spans="1:12">
@@ -719,22 +715,22 @@
         <v>17</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:12">
@@ -858,25 +854,25 @@
     <row r="35" spans="1:12"/>
     <row r="36" spans="1:12">
       <c r="F36" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G36" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G36" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="H36" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="37" spans="1:12">
@@ -995,31 +991,30 @@
       </c>
     </row>
     <row r="42" spans="1:12"/>
-    <row r="43" spans="1:12">
-      <c r="E43" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
+    <row r="43" spans="1:12"/>
     <row r="44" spans="1:12"/>
     <row r="45" spans="1:12"/>
     <row r="46" spans="1:12">
       <c r="F46" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I46" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G46" s="1" t="s">
+      <c r="J46" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H46" s="1" t="s">
+      <c r="K46" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I46" s="1" t="s">
+      <c r="L46" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="J46" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K46" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="47" spans="1:12">
@@ -1041,6 +1036,9 @@
       <c r="K47" t="n">
         <v>0</v>
       </c>
+      <c r="L47" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="48" spans="1:12">
       <c r="F48" s="1" t="s">
@@ -1061,6 +1059,9 @@
       <c r="K48" t="n">
         <v>0</v>
       </c>
+      <c r="L48" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="49" spans="1:12">
       <c r="F49" s="1" t="s">
@@ -1081,6 +1082,9 @@
       <c r="K49" t="n">
         <v>0</v>
       </c>
+      <c r="L49" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="50" spans="1:12">
       <c r="F50" s="1" t="s">
@@ -1101,6 +1105,9 @@
       <c r="K50" t="n">
         <v>0</v>
       </c>
+      <c r="L50" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="51" spans="1:12">
       <c r="F51" s="1" t="s">
@@ -1119,6 +1126,9 @@
         <v>0</v>
       </c>
       <c r="K51" t="n">
+        <v>0</v>
+      </c>
+      <c r="L51" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1181,4 +1191,225 @@
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col customWidth="1" max="1" min="1" width="2.4"/>
+    <col customWidth="1" max="2" min="2" width="2.4"/>
+    <col customWidth="1" max="3" min="3" width="2.4"/>
+    <col customWidth="1" max="4" min="4" width="2.4"/>
+    <col customWidth="1" max="5" min="5" width="34.8"/>
+    <col customWidth="1" max="6" min="6" width="21.6"/>
+    <col customWidth="1" max="7" min="7" width="26.4"/>
+    <col customWidth="1" max="8" min="8" width="12"/>
+    <col customWidth="1" max="9" min="9" width="12"/>
+    <col customWidth="1" max="10" min="10" width="12"/>
+    <col customWidth="1" max="11" min="11" width="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="G1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11"/>
+    <row r="3" spans="1:11">
+      <c r="E3" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11"/>
+    <row r="5" spans="1:11"/>
+    <row r="6" spans="1:11">
+      <c r="F6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="F7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="F8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="F9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="F10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="F11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11"/>
+    <row r="13" spans="1:11">
+      <c r="E13" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11"/>
+    <row r="15" spans="1:11"/>
+    <row r="16" spans="1:11">
+      <c r="F16" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="F17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="F18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="F19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="F20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="F21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>